<commit_message>
Some progress on journal; discussion done.
</commit_message>
<xml_diff>
--- a/510-DistTeams/self_assessment_journal.xlsx
+++ b/510-DistTeams/self_assessment_journal.xlsx
@@ -26,7 +26,404 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+  <si>
+    <r>
+      <t xml:space="preserve">Leadership - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Who's leading and who's not. What does leadership look like?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Membership - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What does it take to be a member of the group? Who is gaining membership, and who is losing it?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Current Thinking</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Thinking</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self Assessment and Development Journal</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Decision Making - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What critical decisions are being made? How are they made?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conflict - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Describe any conflict you see. What does the group do with conflict?</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Turning Points - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Do you see any turning points?  A turning point can be describes as a point in time where the group changes directions, processes etc.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Negative, Limiting &amp; Rational</t>
+  </si>
+  <si>
+    <t>What is This Costing Me?</t>
+  </si>
+  <si>
+    <t>Present Tense, I am…Brief I Specific</t>
+  </si>
+  <si>
+    <t>Conflicts in Team meetings cause discomfort and destroy team moral.</t>
+  </si>
+  <si>
+    <t>New ideas are not heard and solutions to problems not fully explored. I get mediocare solutions</t>
+  </si>
+  <si>
+    <t>I now see that conflicts are natural to groups and it is my job to get all the information I can before making a decsion.</t>
+  </si>
+  <si>
+    <t>We're late.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Panic, rushing through things, stressed.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is really bringing the team together.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>There's too much reading, I'll never keep up</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self-fulfilling</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Come up with a plan. Again.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use these questions to guide your reflection on your thinking. Update the Self Assess Journal tab with the answers to these questions throughout the weeks of the team project.</t>
+  </si>
+  <si>
+    <t>Use these questions to guide your reflection on your thinking about your team. Update the Self Assess Journal tab  with the answers to these questions throughout the weeks of the team project.</t>
+  </si>
+  <si>
+    <t>Use this workbook to capture your weekly journal entries for the Self Assessment Journal assignment. The second tab in this workbook is designed to provide you with a log to capture your journal entries. The second and third tabs – Self Knowledge and Group Dynamics – are suggested questions to get you started or help if you get stuck.  Reflecting can be hard to do, so use these questions and the support of your class and instructor to keep this up. It gets easier with practice. Finally, the last tab contains a few Final Assessment questions and asks you to summarize your journaling in a 1-2 page document. The document and this workbook should be submitted for the Self Assessment assignment in D2L</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What physical sensations accompany this situation?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What images and metaphors come to mind?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What aspects of myself, or my behaviors do I criticize?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What atypical thought patterns are occurring?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What aspects and behaviors of group members do I criticize?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What assumptions do I make about the group or its members?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What expectations do I have about the group or particular members?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Am I resistant to member's suggestions or feedback?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>How do I react to criticism, and in what areas?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>What are my triggers? What seems to arouse my anxiety?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Do I inhibit or encourage self-disclosure in myself or group members?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Where and when do I rationalize?</t>
+    </r>
+  </si>
+  <si>
+    <t>Group Dynamics - Some Questions for Insight</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
   <si>
     <t xml:space="preserve">This log is designed to help you tune your thinking about your own skills and effectiveness as well as that of your team. Start by noting the current thoughts you have on any topic relevant to your experience in your workplace related to teams.  Don’t edit this too much – just write what you think about the situation.
 Next, consider what this type of thinking is “costing” you. Is there a positive or negative impact to this line of thinking?
@@ -115,375 +512,6 @@
   <si>
     <t>What is one skill are where you will continue to focus, in order to be more effective in the future?</t>
     <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>Use these questions to guide your reflection on your thinking. Update the Self Assess Journal tab with the answers to these questions throughout the weeks of the team project.</t>
-  </si>
-  <si>
-    <t>Use these questions to guide your reflection on your thinking about your team. Update the Self Assess Journal tab  with the answers to these questions throughout the weeks of the team project.</t>
-  </si>
-  <si>
-    <t>Use this workbook to capture your weekly journal entries for the Self Assessment Journal assignment. The second tab in this workbook is designed to provide you with a log to capture your journal entries. The second and third tabs – Self Knowledge and Group Dynamics – are suggested questions to get you started or help if you get stuck.  Reflecting can be hard to do, so use these questions and the support of your class and instructor to keep this up. It gets easier with practice. Finally, the last tab contains a few Final Assessment questions and asks you to summarize your journaling in a 1-2 page document. The document and this workbook should be submitted for the Self Assessment assignment in D2L</t>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What physical sensations accompany this situation?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What images and metaphors come to mind?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What aspects of myself, or my behaviors do I criticize?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What atypical thought patterns are occurring?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What aspects and behaviors of group members do I criticize?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What assumptions do I make about the group or its members?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What expectations do I have about the group or particular members?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Am I resistant to member's suggestions or feedback?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>How do I react to criticism, and in what areas?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What are my triggers? What seems to arouse my anxiety?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Do I inhibit or encourage self-disclosure in myself or group members?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Where and when do I rationalize?</t>
-    </r>
-  </si>
-  <si>
-    <t>Group Dynamics - Some Questions for Insight</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Leadership - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Who's leading and who's not. What does leadership look like?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Membership - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What does it take to be a member of the group? Who is gaining membership, and who is losing it?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Current Thinking</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>New Thinking</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self Assessment and Development Journal</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Decision Making - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>What critical decisions are being made? How are they made?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Conflict - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Describe any conflict you see. What does the group do with conflict?</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Turning Points - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Do you see any turning points?  A turning point can be describes as a point in time where the group changes directions, processes etc.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Negative, Limiting &amp; Rational</t>
-  </si>
-  <si>
-    <t>What is This Costing Me?</t>
-  </si>
-  <si>
-    <t>Present Tense, I am…Brief I Specific</t>
-  </si>
-  <si>
-    <t>Conflicts in Team meetings cause discomfort and destroy team moral.</t>
-  </si>
-  <si>
-    <t>New ideas are not heard and solutions to problems not fully explored. I get mediocare solutions</t>
-  </si>
-  <si>
-    <t>I now see that conflicts are natural to groups and it is my job to get all the information I can before making a decsion.</t>
   </si>
 </sst>
 </file>
@@ -553,12 +581,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -582,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -604,13 +638,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -638,12 +665,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,8 +1060,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="75">
-      <c r="A1" s="22" t="s">
-        <v>18</v>
+      <c r="A1" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1042,8 +1083,8 @@
   </sheetPr>
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
@@ -1055,83 +1096,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17">
-      <c r="B1" s="20" t="s">
-        <v>36</v>
+      <c r="B1" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="4"/>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="99" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="5" spans="1:4" ht="15">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13" thickBot="1">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5" thickTop="1"/>
-    <row r="8" spans="1:4" s="11" customFormat="1" ht="24">
-      <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+    <row r="8" spans="1:4" s="24" customFormat="1" ht="24">
+      <c r="A8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="27" customFormat="1">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" ht="24">
       <c r="A10" s="7">
         <v>40557</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>3</v>
+        <v>41</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1145,23 +1186,33 @@
         <v>40565</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="24">
+      <c r="A13" s="7">
+        <v>40570</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1177,10 +1228,18 @@
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="7">
+        <v>40604</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7"/>
@@ -1443,120 +1502,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
-      <c r="A1" s="12" t="s">
-        <v>10</v>
+      <c r="A1" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18">
-      <c r="A2" s="12"/>
+      <c r="A2" s="9"/>
     </row>
     <row r="3" spans="1:1" ht="48">
-      <c r="A3" s="16" t="s">
-        <v>16</v>
+      <c r="A3" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18">
-      <c r="A4" s="12"/>
+      <c r="A4" s="9"/>
     </row>
     <row r="5" spans="1:1" ht="16">
-      <c r="A5" s="14" t="s">
-        <v>11</v>
+      <c r="A5" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15">
-      <c r="A6" s="13"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1" ht="16">
-      <c r="A7" s="14" t="s">
-        <v>19</v>
+      <c r="A7" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15">
-      <c r="A8" s="13"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:1" ht="16">
-      <c r="A9" s="14" t="s">
-        <v>20</v>
+      <c r="A9" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15">
-      <c r="A10" s="13"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:1" ht="16">
-      <c r="A11" s="14" t="s">
-        <v>21</v>
+      <c r="A11" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15">
-      <c r="A12" s="13"/>
+      <c r="A12" s="10"/>
     </row>
     <row r="13" spans="1:1" ht="16">
-      <c r="A13" s="14" t="s">
-        <v>22</v>
+      <c r="A13" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15">
-      <c r="A14" s="13"/>
+      <c r="A14" s="10"/>
     </row>
     <row r="15" spans="1:1" ht="16">
-      <c r="A15" s="14" t="s">
-        <v>23</v>
+      <c r="A15" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15">
-      <c r="A16" s="13"/>
+      <c r="A16" s="10"/>
     </row>
     <row r="17" spans="1:1" ht="16">
-      <c r="A17" s="14" t="s">
-        <v>24</v>
+      <c r="A17" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15">
-      <c r="A18" s="13"/>
+      <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:1" ht="16">
-      <c r="A19" s="14" t="s">
-        <v>25</v>
+      <c r="A19" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15">
-      <c r="A20" s="13"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" ht="16">
-      <c r="A21" s="14" t="s">
-        <v>26</v>
+      <c r="A21" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15">
-      <c r="A22" s="13"/>
+      <c r="A22" s="10"/>
     </row>
     <row r="23" spans="1:1" ht="16">
-      <c r="A23" s="14" t="s">
-        <v>27</v>
+      <c r="A23" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15">
-      <c r="A24" s="13"/>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:1" ht="16">
-      <c r="A25" s="14" t="s">
-        <v>28</v>
+      <c r="A25" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15">
-      <c r="A26" s="13"/>
+      <c r="A26" s="10"/>
     </row>
     <row r="27" spans="1:1" ht="16">
-      <c r="A27" s="14" t="s">
-        <v>29</v>
+      <c r="A27" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15">
-      <c r="A28" s="13"/>
+      <c r="A28" s="10"/>
     </row>
     <row r="29" spans="1:1" ht="16">
-      <c r="A29" s="14" t="s">
-        <v>30</v>
+      <c r="A29" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1586,38 +1645,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
-      <c r="A1" s="15" t="s">
-        <v>31</v>
+      <c r="A1" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="32">
-      <c r="A3" s="16" t="s">
-        <v>17</v>
+      <c r="A3" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18">
-      <c r="A5" s="15" t="s">
-        <v>32</v>
+      <c r="A5" s="12" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="36">
-      <c r="A7" s="15" t="s">
-        <v>33</v>
+      <c r="A7" s="12" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18">
-      <c r="A9" s="15" t="s">
-        <v>37</v>
+      <c r="A9" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18">
-      <c r="A11" s="15" t="s">
-        <v>38</v>
+      <c r="A11" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="36">
-      <c r="A13" s="15" t="s">
-        <v>39</v>
+      <c r="A13" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1647,37 +1706,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="21" t="s">
-        <v>12</v>
+      <c r="A1" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:1" ht="24">
-      <c r="A3" s="17" t="s">
-        <v>13</v>
+      <c r="A3" s="14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="18"/>
+      <c r="A4" s="15"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="17" t="s">
-        <v>14</v>
+      <c r="A5" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="19"/>
+      <c r="A6" s="16"/>
     </row>
     <row r="7" spans="1:1" ht="24">
-      <c r="A7" s="17" t="s">
-        <v>15</v>
+      <c r="A7" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="36">
       <c r="A10" s="3" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>